<commit_message>
bibliography and cv updated
</commit_message>
<xml_diff>
--- a/tables/portfolio.xlsx
+++ b/tables/portfolio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4877c03b8c303747/Desktop/thesis_bookdown/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{E211F4C2-8F67-4FCD-A3E4-DC64A70892F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D7A8591-A9A1-42FE-B7AF-BA8D014948FC}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="8_{E211F4C2-8F67-4FCD-A3E4-DC64A70892F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{891BD08C-D9A1-4B23-AFE9-C37DFA7038F6}"/>
   <bookViews>
     <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{5DF30DC9-9093-4DAD-A9AD-849867C6675C}"/>
   </bookViews>
@@ -51,9 +51,6 @@
     <t>EP16 - Missing Values in Clinical Research (NIHES)</t>
   </si>
   <si>
-    <t>RaukR. Advanced R for Bioinformatics Summer School (Visby, Sweden)</t>
-  </si>
-  <si>
     <t>CE08 - Repeated Measurements (NIHES)</t>
   </si>
   <si>
@@ -159,9 +156,6 @@
     <t>ECTS*</t>
   </si>
   <si>
-    <t>Peer-review</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -175,14 +169,51 @@
   </si>
   <si>
     <t>O</t>
+  </si>
+  <si>
+    <r>
+      <t>RaukR: Advanced R for Bioinformatics Summer School (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SciLifeLab</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Peer-review: Epidemiology, European Journal of Epidemiology, Journal of Causal Inference,  BMC Medical Research Methodology, Plos One, The American Journal of Drug and Alcohol Abuse, Journal of the Intensive Care Society</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -532,7 +563,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:XFD30"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -548,10 +579,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
         <v>40</v>
-      </c>
-      <c r="D1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -565,7 +596,7 @@
         <v>1.4</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -579,7 +610,7 @@
         <v>1.4</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -593,12 +624,12 @@
         <v>1.7</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="B5">
         <v>2019</v>
@@ -607,12 +638,12 @@
         <v>2.4</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>2019</v>
@@ -621,12 +652,12 @@
         <v>1.7</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>2019</v>
@@ -635,12 +666,12 @@
         <v>0.7</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>2020</v>
@@ -649,12 +680,12 @@
         <v>3.4</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>2021</v>
@@ -663,12 +694,12 @@
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>2021</v>
@@ -679,7 +710,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>2020</v>
@@ -688,12 +719,12 @@
         <v>1.2</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>2020</v>
@@ -702,12 +733,12 @@
         <v>1.2</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>2020</v>
@@ -716,12 +747,12 @@
         <v>1.2</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>2020</v>
@@ -730,12 +761,12 @@
         <v>1.2</v>
       </c>
       <c r="D14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>2021</v>
@@ -744,12 +775,12 @@
         <v>1.2</v>
       </c>
       <c r="D15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16">
         <v>2021</v>
@@ -758,20 +789,20 @@
         <v>1.8</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18">
         <v>2019</v>
@@ -780,26 +811,26 @@
         <v>1.4</v>
       </c>
       <c r="D18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20">
         <v>2020</v>
@@ -808,94 +839,94 @@
         <v>1.4</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22">
         <v>2021</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23">
         <v>2020</v>
       </c>
       <c r="D23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24">
         <v>2020</v>
       </c>
       <c r="D24" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25">
         <v>2020</v>
       </c>
       <c r="D25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26">
         <v>2019</v>
       </c>
       <c r="D26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27">
         <v>2019</v>
       </c>
       <c r="D27" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29">
         <v>2020</v>
@@ -904,95 +935,95 @@
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C30">
         <v>1.6</v>
       </c>
       <c r="D30" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D31" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32">
         <v>2019</v>
       </c>
       <c r="D32" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33">
         <v>2018</v>
       </c>
       <c r="D33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D34" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C35">
         <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D36" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
         <v>36</v>
       </c>
-      <c r="B37" t="s">
-        <v>37</v>
-      </c>
       <c r="D37" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
detalles cap 4 al 10 listoo; detalles tablas sup chap 3 tb
</commit_message>
<xml_diff>
--- a/tables/portfolio.xlsx
+++ b/tables/portfolio.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4877c03b8c303747/Desktop/thesis_bookdown/tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4877c03b8c303747/Desktop/tables_test/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="8_{E211F4C2-8F67-4FCD-A3E4-DC64A70892F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{891BD08C-D9A1-4B23-AFE9-C37DFA7038F6}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="8_{E211F4C2-8F67-4FCD-A3E4-DC64A70892F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{270D1169-3B3D-4272-883D-E64400105A47}"/>
   <bookViews>
     <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{5DF30DC9-9093-4DAD-A9AD-849867C6675C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="48">
   <si>
     <t>Activity</t>
   </si>
@@ -197,7 +197,10 @@
     </r>
   </si>
   <si>
-    <t>Peer-review: Epidemiology, European Journal of Epidemiology, Journal of Causal Inference,  BMC Medical Research Methodology, Plos One, The American Journal of Drug and Alcohol Abuse, Journal of the Intensive Care Society</t>
+    <t>Epidemiology, European Journal of Epidemiology, Journal of Causal Inference,  BMC Medical Research Methodology, Plos One, The American Journal of Drug and Alcohol Abuse, Journal of the Intensive Care Society</t>
+  </si>
+  <si>
+    <t>Peer Review</t>
   </si>
 </sst>
 </file>
@@ -560,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE3A92B6-8D7C-46CC-848A-7417F6E20566}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -940,13 +943,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>46</v>
-      </c>
-      <c r="B30" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30">
-        <v>1.6</v>
+        <v>47</v>
       </c>
       <c r="D30" t="s">
         <v>44</v>
@@ -954,7 +951,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>46</v>
+      </c>
+      <c r="B31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31">
+        <v>1.6</v>
       </c>
       <c r="D31" t="s">
         <v>44</v>
@@ -962,10 +965,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>28</v>
-      </c>
-      <c r="B32">
-        <v>2019</v>
+        <v>29</v>
       </c>
       <c r="D32" t="s">
         <v>44</v>
@@ -973,10 +973,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B33">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="D33" t="s">
         <v>44</v>
@@ -984,7 +984,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>30</v>
+      </c>
+      <c r="B34">
+        <v>2018</v>
       </c>
       <c r="D34" t="s">
         <v>44</v>
@@ -992,13 +995,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C35">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="D35" t="s">
         <v>44</v>
@@ -1006,10 +1003,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>20</v>
+        <v>33</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
       </c>
       <c r="D36" t="s">
         <v>44</v>
@@ -1017,12 +1017,23 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>35</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>36</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ordenar por fecha de menor a mayor
</commit_message>
<xml_diff>
--- a/tables/portfolio.xlsx
+++ b/tables/portfolio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4877c03b8c303747/Desktop/tables_test/tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4877c03b8c303747/Desktop/thesis_bookdown/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="8_{E211F4C2-8F67-4FCD-A3E4-DC64A70892F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{270D1169-3B3D-4272-883D-E64400105A47}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="8_{E211F4C2-8F67-4FCD-A3E4-DC64A70892F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9A52126-058E-4CE9-8B3F-450F3DEB20EA}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{5DF30DC9-9093-4DAD-A9AD-849867C6675C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5DF30DC9-9093-4DAD-A9AD-849867C6675C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -565,13 +565,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE3A92B6-8D7C-46CC-848A-7417F6E20566}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="157" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D33" sqref="A28:D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -855,10 +856,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B22">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="D22" t="s">
         <v>43</v>
@@ -866,10 +867,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B23">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D23" t="s">
         <v>43</v>
@@ -877,7 +878,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24">
         <v>2020</v>
@@ -888,7 +889,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>2020</v>
@@ -899,10 +900,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B26">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="D26" t="s">
         <v>43</v>
@@ -910,10 +911,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B27">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="D27" t="s">
         <v>43</v>
@@ -973,10 +974,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B33">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D33" t="s">
         <v>44</v>
@@ -984,10 +985,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B34">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="D34" t="s">
         <v>44</v>
@@ -1003,13 +1004,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>33</v>
-      </c>
-      <c r="C36">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="D36" t="s">
         <v>44</v>
@@ -1028,10 +1026,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
       </c>
       <c r="D38" t="s">
         <v>44</v>

</xml_diff>